<commit_message>
minor changes to user stories doc
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KATALYTIC\Desktop\Work\Uni\Second Year\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Games\Documents\GitHub\mgp-mgp-group-13\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B4C9DA-7722-426C-B995-1F899550F467}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>User Story</t>
   </si>
@@ -271,12 +270,27 @@
   </si>
   <si>
     <t>Implement collision for jellyfish (no user input should be required)</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>cerate new input system to allow players to use a powerup witout using a turn</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>display this score as an image based tally</t>
+  </si>
+  <si>
+    <t>animation system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,23 +506,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -544,23 +541,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -736,18 +716,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="81.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="51.42578125" customWidth="1"/>
   </cols>
@@ -783,6 +763,9 @@
       <c r="C4" t="s">
         <v>74</v>
       </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
       <c r="J4" t="s">
         <v>71</v>
       </c>
@@ -791,21 +774,19 @@
       <c r="C5" t="s">
         <v>79</v>
       </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
       <c r="J5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="J6" t="s">
-        <v>73</v>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -813,257 +794,274 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>77</v>
+        <v>82</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>1</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>1</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>1</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>80</v>
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>75</v>
-      </c>
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>1</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>41</v>
-      </c>
+      <c r="A39" s="6">
+        <v>1</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
-        <v>1</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>2</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>2</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>2</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>2</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>2</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -1073,14 +1071,14 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,191 +1086,206 @@
         <v>2</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>2</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
-        <v>2</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>47</v>
-      </c>
+      <c r="A61" s="6">
+        <v>2</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6">
-        <v>2</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>58</v>
-      </c>
+      <c r="A68" s="6">
+        <v>2</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="6">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
         <v>3</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="6">
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
         <v>3</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
         <v>1</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B129" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C127" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C131" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1283,7 +1296,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1295,7 +1308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated documentation to show remaining tasks
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Year 2\Group Project\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF082E13-F610-4509-B1E5-3CDB87AE04D5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
   <si>
     <t>User Story</t>
   </si>
@@ -376,8 +370,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,7 +383,18 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -401,13 +406,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor indexed="31"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,15 +466,6 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -479,6 +475,15 @@
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -494,29 +499,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -563,7 +560,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,27 +592,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -647,24 +626,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -840,28 +801,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="87" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="5"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -873,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickTop="1">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -883,7 +843,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" t="s">
         <v>65</v>
       </c>
@@ -894,7 +854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" t="s">
         <v>70</v>
       </c>
@@ -905,7 +865,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="C6" t="s">
         <v>76</v>
       </c>
@@ -916,7 +876,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" t="s">
         <v>91</v>
       </c>
@@ -924,7 +884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -934,7 +894,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -944,7 +904,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -954,7 +914,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="C11" t="s">
         <v>72</v>
       </c>
@@ -962,15 +922,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="C12" t="s">
         <v>80</v>
       </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
       <c r="E12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -980,7 +943,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="C14" t="s">
         <v>36</v>
       </c>
@@ -988,7 +951,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="C15" t="s">
         <v>73</v>
       </c>
@@ -996,7 +959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -1006,7 +969,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="C17" t="s">
         <v>67</v>
       </c>
@@ -1014,7 +977,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="C18" t="s">
         <v>68</v>
       </c>
@@ -1022,7 +985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="C19" t="s">
         <v>69</v>
       </c>
@@ -1030,7 +993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="C20" t="s">
         <v>33</v>
       </c>
@@ -1038,7 +1001,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="C21" t="s">
         <v>34</v>
       </c>
@@ -1046,19 +1009,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="C22" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" t="s">
         <v>93</v>
       </c>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -1074,45 +1036,43 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="C24" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" t="s">
         <v>96</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="C25" t="s">
         <v>26</v>
       </c>
       <c r="D25" t="s">
         <v>74</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" t="s">
         <v>97</v>
       </c>
-      <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11">
       <c r="C26" t="s">
         <v>28</v>
       </c>
       <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" t="s">
         <v>98</v>
       </c>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="6">
         <v>1</v>
       </c>
@@ -1121,102 +1081,99 @@
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="J27" s="8" t="s">
+      <c r="J27" t="s">
         <v>99</v>
       </c>
-      <c r="K27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11">
       <c r="C28" t="s">
         <v>42</v>
       </c>
       <c r="E28" t="s">
         <v>113</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" t="s">
         <v>100</v>
       </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11">
       <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" t="s">
         <v>113</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" t="s">
         <v>101</v>
       </c>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11">
       <c r="C30" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" t="s">
         <v>113</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" t="s">
         <v>102</v>
       </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11">
       <c r="C31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" t="s">
         <v>113</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11">
       <c r="C32" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" t="s">
         <v>113</v>
       </c>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10">
       <c r="C33" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" t="s">
         <v>113</v>
       </c>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10">
       <c r="C34" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
         <v>113</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" t="s">
         <v>103</v>
       </c>
-      <c r="K34" s="8"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10">
       <c r="C35" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
         <v>113</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" t="s">
         <v>104</v>
       </c>
-      <c r="K35" s="8"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -1226,7 +1183,7 @@
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="C37" t="s">
         <v>43</v>
       </c>
@@ -1234,31 +1191,40 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="C38" t="s">
         <v>44</v>
       </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
       <c r="E38" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="C39" t="s">
         <v>45</v>
       </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
       <c r="E39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="C40" t="s">
         <v>46</v>
       </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
       <c r="E40" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="C41" t="s">
         <v>59</v>
       </c>
@@ -1266,7 +1232,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="C42" t="s">
         <v>60</v>
       </c>
@@ -1274,7 +1240,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="6">
         <v>1</v>
       </c>
@@ -1284,7 +1250,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="C44" t="s">
         <v>30</v>
       </c>
@@ -1292,7 +1258,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="C45" t="s">
         <v>71</v>
       </c>
@@ -1300,7 +1266,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="C46" t="s">
         <v>66</v>
       </c>
@@ -1308,7 +1274,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="C47" t="s">
         <v>31</v>
       </c>
@@ -1316,7 +1282,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="C48" t="s">
         <v>37</v>
       </c>
@@ -1324,7 +1290,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="6">
         <v>1</v>
       </c>
@@ -1334,7 +1300,7 @@
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="C50" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="C51" t="s">
         <v>38</v>
       </c>
@@ -1350,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="C52" t="s">
         <v>110</v>
       </c>
@@ -1358,7 +1324,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="C53" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1332,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="C54" t="s">
         <v>41</v>
       </c>
@@ -1374,27 +1340,27 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="C55" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="C56" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="C57" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="C58" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="6">
         <v>1</v>
       </c>
@@ -1404,7 +1370,7 @@
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="6">
         <v>2</v>
       </c>
@@ -1414,7 +1380,7 @@
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="6">
         <v>2</v>
       </c>
@@ -1424,7 +1390,7 @@
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="6">
         <v>2</v>
       </c>
@@ -1434,7 +1400,7 @@
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="6">
         <v>2</v>
       </c>
@@ -1444,12 +1410,12 @@
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="C64" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="6">
         <v>2</v>
       </c>
@@ -1459,7 +1425,7 @@
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="C66" t="s">
         <v>29</v>
       </c>
@@ -1467,7 +1433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="6">
         <v>2</v>
       </c>
@@ -1477,7 +1443,7 @@
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="C68" t="s">
         <v>32</v>
       </c>
@@ -1485,7 +1451,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="C69" t="s">
         <v>30</v>
       </c>
@@ -1493,7 +1459,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="C70" t="s">
         <v>88</v>
       </c>
@@ -1501,7 +1467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="C71" t="s">
         <v>89</v>
       </c>
@@ -1509,12 +1475,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="C72" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="6">
         <v>2</v>
       </c>
@@ -1527,42 +1496,54 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="C74" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="C75" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="C76" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="C77" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="C78" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="C79" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="C80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="6">
         <v>2</v>
       </c>
@@ -1575,77 +1556,77 @@
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="C82" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="C83" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="C84" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="C85" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="C86" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="C87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="C88" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="C89" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="C90" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="C91" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="C92" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="C93" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="C94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="C95" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="6">
         <v>3</v>
       </c>
@@ -1655,7 +1636,7 @@
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="6">
         <v>3</v>
       </c>
@@ -1666,7 +1647,8 @@
       <c r="D97" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>